<commit_message>
Testing for "Sign-In" Complete. All tests passed. (Sign-Out left in list but marked accordingly)
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\Desktop\team-project-2185-swen-261-10-b\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58611D2-9C3C-4FB5-949B-91478767D982}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4320" windowWidth="18705" windowHeight="7545" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Instructions</t>
   </si>
@@ -118,12 +124,18 @@
 Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers.xslx.
 Submit this file per the instructions specified for the sprint submissions, cross-team testing, and Freshman Seminar testing.</t>
   </si>
+  <si>
+    <t>**ACCEPTANCE CRITERIA MOVED TO SPRINT 2**</t>
+  </si>
+  <si>
+    <t>JS (3/1)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,13 +164,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -179,10 +215,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -218,98 +256,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -349,13 +312,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -375,93 +331,14 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -788,11 +665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -836,12 +713,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H599"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="topRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -883,86 +760,113 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="8"/>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="8"/>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8"/>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="8"/>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="8"/>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="8"/>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
+      <c r="B8" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="8"/>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="8"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
+      <c r="B10" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="8"/>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="G10" s="8"/>
     </row>
@@ -3952,39 +3856,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D599">
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>AND(ISBLANK(D2),C2="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
-      <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F599">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H599">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E599 C2:C599 G2:G599">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E599 C2:C599 G2:G599" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>